<commit_message>
Rename sheet in all_classes
</commit_message>
<xml_diff>
--- a/AllClasses.xlsx
+++ b/AllClasses.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="import" sheetId="2" r:id="rId1"/>
-    <sheet name="export" sheetId="1" r:id="rId2"/>
+    <sheet name="export" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,10 +26,13 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="ClassesSample" type="4" refreshedVersion="0" background="1">
+  <connection id="1" name="AllClasses" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\MiSc\Desktop\MyFTV\Notes\Meta\AllClasses.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="2" name="ClassesSample" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\MiSc\Desktop\MyFTV\Notes\Meta\ClassesSample.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" name="model" type="4" refreshedVersion="0" background="1">
+  <connection id="3" name="model" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\MiSc\Desktop\MyFTV\Notes\Meta\model.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -1484,28 +1487,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1519,104 +1501,10 @@
 </file>
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
-<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="xmlns:ns1='http://www.eclipse.org/uml2/5.0.0/UML' xmlns:ns2='http://www.omg.org/spec/XMI/20131001'">
-  <Schema ID="Schema1" Namespace="http://www.omg.org/spec/XMI/20131001">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:ns0="http://www.omg.org/spec/XMI/20131001" xmlns="" targetNamespace="http://www.omg.org/spec/XMI/20131001">
-      <xsd:attribute name="version" type="xsd:integer"/>
-      <xsd:attribute name="id" type="xsd:string"/>
-      <xsd:attribute name="type" type="xsd:string"/>
-    </xsd:schema>
-  </Schema>
-  <Schema ID="Schema2">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:ns0="http://www.omg.org/spec/XMI/20131001" xmlns="">
-      <xsd:import namespace="http://www.omg.org/spec/XMI/20131001"/>
-      <xsd:element nillable="true" name="packagedElement">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0" maxOccurs="unbounded">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="ownedAttribute" form="unqualified">
-              <xsd:complexType>
-                <xsd:attribute ref="ns0:type"/>
-                <xsd:attribute ref="ns0:id"/>
-                <xsd:attribute name="name" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="type" form="unqualified" type="xsd:string"/>
-              </xsd:complexType>
-            </xsd:element>
-            <xsd:element minOccurs="0" nillable="true" name="generalization" form="unqualified">
-              <xsd:complexType>
-                <xsd:attribute ref="ns0:type"/>
-                <xsd:attribute ref="ns0:id"/>
-                <xsd:attribute name="general" form="unqualified" type="xsd:string"/>
-              </xsd:complexType>
-            </xsd:element>
-            <xsd:element minOccurs="0" nillable="true" name="eAnnotations" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" name="details" form="unqualified">
-                    <xsd:complexType>
-                      <xsd:attribute ref="ns0:type"/>
-                      <xsd:attribute ref="ns0:id"/>
-                      <xsd:attribute name="key" form="unqualified" type="xsd:string"/>
-                      <xsd:attribute name="value" form="unqualified" type="xsd:string"/>
-                    </xsd:complexType>
-                  </xsd:element>
-                </xsd:sequence>
-                <xsd:attribute ref="ns0:type"/>
-                <xsd:attribute ref="ns0:id"/>
-                <xsd:attribute name="source" form="unqualified" type="xsd:string"/>
-              </xsd:complexType>
-            </xsd:element>
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="ownedEnd" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" name="lowerValue" form="unqualified">
-                    <xsd:complexType>
-                      <xsd:attribute ref="ns0:type"/>
-                      <xsd:attribute ref="ns0:id"/>
-                    </xsd:complexType>
-                  </xsd:element>
-                  <xsd:element minOccurs="0" nillable="true" name="upperValue" form="unqualified">
-                    <xsd:complexType>
-                      <xsd:attribute ref="ns0:type"/>
-                      <xsd:attribute ref="ns0:id"/>
-                      <xsd:attribute name="value" form="unqualified" type="xsd:string"/>
-                    </xsd:complexType>
-                  </xsd:element>
-                </xsd:sequence>
-                <xsd:attribute ref="ns0:type"/>
-                <xsd:attribute ref="ns0:id"/>
-                <xsd:attribute name="name" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="type" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="association" form="unqualified" type="xsd:string"/>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-          <xsd:attribute ref="ns0:type"/>
-          <xsd:attribute ref="ns0:id"/>
-          <xsd:attribute name="name" form="unqualified" type="xsd:string"/>
-          <xsd:attribute name="memberEnd" form="unqualified" type="xsd:string"/>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Schema ID="Schema3" SchemaRef="Schema1 Schema2" Namespace="http://www.eclipse.org/uml2/5.0.0/UML">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:ns0="http://www.omg.org/spec/XMI/20131001" xmlns:ns1="http://www.eclipse.org/uml2/5.0.0/UML" xmlns="" targetNamespace="http://www.eclipse.org/uml2/5.0.0/UML">
-      <xsd:import namespace="http://www.omg.org/spec/XMI/20131001"/>
-      <xsd:import/>
-      <xsd:element nillable="true" name="Model">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" ref="packagedElement"/>
-          </xsd:sequence>
-          <xsd:attribute ref="ns0:version"/>
-          <xsd:attribute ref="ns0:id"/>
-          <xsd:attribute name="name" form="unqualified" type="xsd:string"/>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Schema ID="Schema4">
+<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
+  <Schema ID="Schema5">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="sheet">
+      <xsd:element nillable="true" name="all_classes">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
             <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="class" form="unqualified">
@@ -1624,7 +1512,7 @@
                 <xsd:sequence minOccurs="0">
                   <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="name" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="id" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="base" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="base" form="unqualified"/>
                 </xsd:sequence>
               </xsd:complexType>
             </xsd:element>
@@ -1633,30 +1521,27 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="1" Name="Model_Map" RootElement="Model" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
-  </Map>
-  <Map ID="2" Name="sheet_Map" RootElement="sheet" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+  <Map ID="3" Name="all_classes_Map" RootElement="all_classes" SchemaID="Schema5" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding DataBindingName="Binding1" FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C461" tableType="xml" totalsRowShown="0" headerRowDxfId="1" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C461" tableType="xml" totalsRowShown="0" connectionId="1">
   <autoFilter ref="A1:C461"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="name" name="name">
       <calculatedColumnFormula>import!$A2</calculatedColumnFormula>
-      <xmlColumnPr mapId="2" xpath="/sheet/class/name" xmlDataType="string"/>
+      <xmlColumnPr mapId="3" xpath="/all_classes/class/name" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="id" name="id">
       <calculatedColumnFormula>import!C2</calculatedColumnFormula>
-      <xmlColumnPr mapId="2" xpath="/sheet/class/id" xmlDataType="integer"/>
+      <xmlColumnPr mapId="3" xpath="/all_classes/class/id" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="base" name="base" dataDxfId="0">
+    <tableColumn id="3" uniqueName="base" name="base">
       <calculatedColumnFormula>import!D2</calculatedColumnFormula>
-      <xmlColumnPr mapId="2" xpath="/sheet/class/base" xmlDataType="integer"/>
+      <xmlColumnPr mapId="3" xpath="/all_classes/class/base" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1929,7 +1814,7 @@
   <dimension ref="A1:D461"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A437" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -9316,26 +9201,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C461"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C461"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="3" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -15781,9 +15664,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>